<commit_message>
DOC - 2-pin CON cost update
</commit_message>
<xml_diff>
--- a/1_Schematic/V2.0/Plasma Generator_Part List_V2.0_20171222.xlsx
+++ b/1_Schematic/V2.0/Plasma Generator_Part List_V2.0_20171222.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="266">
   <si>
     <t>No</t>
   </si>
@@ -652,10 +652,6 @@
   </si>
   <si>
     <t>LM2735XMF</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
-    <t>12512WS-04B</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
@@ -941,6 +937,14 @@
   <si>
     <t>R1, R3, R7, R9, R11, R12, R13, R14, R18, R20,
 R21, R28, R31, R32, R33, R34, R42</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>12512WS-02B</t>
+    <phoneticPr fontId="22" type="noConversion"/>
+  </si>
+  <si>
+    <t>12512WS-04B</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -2247,11 +2251,11 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="48">
@@ -2585,9 +2589,9 @@
   </sheetPr>
   <dimension ref="A1:X61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2631,10 +2635,10 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C3" s="102" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H3" s="55" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="T3" s="15" t="s">
         <v>182</v>
@@ -2678,10 +2682,10 @@
         <v>6</v>
       </c>
       <c r="H5" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="I5" s="25" t="s">
         <v>235</v>
-      </c>
-      <c r="I5" s="25" t="s">
-        <v>236</v>
       </c>
       <c r="J5" s="25" t="s">
         <v>7</v>
@@ -2888,7 +2892,7 @@
       </c>
       <c r="I8" s="53"/>
       <c r="J8" s="85" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K8" s="53" t="s">
         <v>21</v>
@@ -2955,7 +2959,7 @@
       </c>
       <c r="I9" s="53"/>
       <c r="J9" s="52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K9" s="19" t="s">
         <v>21</v>
@@ -3020,7 +3024,7 @@
       </c>
       <c r="I10" s="53"/>
       <c r="J10" s="52" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="K10" s="19" t="s">
         <v>16</v>
@@ -3154,7 +3158,7 @@
       </c>
       <c r="I12" s="53"/>
       <c r="J12" s="83" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K12" s="53" t="s">
         <v>21</v>
@@ -3221,7 +3225,7 @@
       </c>
       <c r="I13" s="53"/>
       <c r="J13" s="52" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K13" s="19" t="s">
         <v>21</v>
@@ -3274,10 +3278,10 @@
         <v>34</v>
       </c>
       <c r="E14" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="F14" s="27" t="s">
         <v>239</v>
-      </c>
-      <c r="F14" s="27" t="s">
-        <v>240</v>
       </c>
       <c r="G14" s="56">
         <v>4</v>
@@ -3288,7 +3292,7 @@
       </c>
       <c r="I14" s="53"/>
       <c r="J14" s="27" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K14" s="19" t="s">
         <v>21</v>
@@ -3355,7 +3359,7 @@
       </c>
       <c r="I15" s="53"/>
       <c r="J15" s="27" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K15" s="19" t="s">
         <v>21</v>
@@ -3536,16 +3540,16 @@
         <v>13</v>
       </c>
       <c r="C18" s="53" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D18" s="53" t="s">
         <v>34</v>
       </c>
       <c r="E18" s="52" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F18" s="52" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G18" s="74">
         <v>17</v>
@@ -3556,7 +3560,7 @@
       </c>
       <c r="I18" s="53"/>
       <c r="J18" s="57" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K18" s="53" t="s">
         <v>21</v>
@@ -3670,16 +3674,16 @@
         <v>15</v>
       </c>
       <c r="C20" s="56" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D20" s="56" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="F20" s="27" t="s">
         <v>243</v>
-      </c>
-      <c r="F20" s="27" t="s">
-        <v>244</v>
       </c>
       <c r="G20" s="53">
         <v>1</v>
@@ -3690,7 +3694,7 @@
       </c>
       <c r="I20" s="53"/>
       <c r="J20" s="27" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K20" s="19" t="s">
         <v>21</v>
@@ -3955,16 +3959,16 @@
         <v>19</v>
       </c>
       <c r="C24" s="53" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D24" s="53" t="s">
+        <v>211</v>
+      </c>
+      <c r="E24" s="47" t="s">
+        <v>210</v>
+      </c>
+      <c r="F24" s="52" t="s">
         <v>212</v>
-      </c>
-      <c r="E24" s="47" t="s">
-        <v>211</v>
-      </c>
-      <c r="F24" s="52" t="s">
-        <v>213</v>
       </c>
       <c r="G24" s="53">
         <v>1</v>
@@ -3978,10 +3982,10 @@
         <v>68</v>
       </c>
       <c r="K24" s="53" t="s">
+        <v>213</v>
+      </c>
+      <c r="L24" s="50" t="s">
         <v>214</v>
-      </c>
-      <c r="L24" s="50" t="s">
-        <v>215</v>
       </c>
       <c r="M24" s="48">
         <v>1990</v>
@@ -3998,10 +4002,10 @@
         <v>1990</v>
       </c>
       <c r="Q24" s="47" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="R24" s="47" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="S24" s="62" t="s">
         <v>138</v>
@@ -4191,7 +4195,7 @@
         <v>10</v>
       </c>
       <c r="J27" s="51" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K27" s="53" t="s">
         <v>83</v>
@@ -4239,7 +4243,7 @@
         <v>23</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>85</v>
@@ -4381,16 +4385,16 @@
         <v>25</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>97</v>
       </c>
       <c r="E30" s="84" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F30" s="52" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G30" s="53">
         <v>1</v>
@@ -4593,7 +4597,7 @@
         <v>28</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D33" s="19" t="s">
         <v>112</v>
@@ -4665,7 +4669,7 @@
         <v>29</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>192</v>
+        <v>265</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>117</v>
@@ -4739,16 +4743,16 @@
         <v>30</v>
       </c>
       <c r="C35" s="53" t="s">
+        <v>224</v>
+      </c>
+      <c r="D35" s="53" t="s">
         <v>225</v>
       </c>
-      <c r="D35" s="53" t="s">
+      <c r="E35" s="47" t="s">
         <v>226</v>
       </c>
-      <c r="E35" s="47" t="s">
-        <v>227</v>
-      </c>
       <c r="F35" s="52" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G35" s="53">
         <v>1</v>
@@ -4762,10 +4766,10 @@
         <v>122</v>
       </c>
       <c r="K35" s="53" t="s">
+        <v>227</v>
+      </c>
+      <c r="L35" s="50" t="s">
         <v>228</v>
-      </c>
-      <c r="L35" s="50" t="s">
-        <v>229</v>
       </c>
       <c r="M35" s="48">
         <v>320</v>
@@ -4782,10 +4786,10 @@
         <v>320</v>
       </c>
       <c r="Q35" s="52" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="R35" s="49" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S35" s="62" t="s">
         <v>138</v>
@@ -4811,7 +4815,7 @@
         <v>31</v>
       </c>
       <c r="C36" s="53" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D36" s="53" t="s">
         <v>124</v>
@@ -4820,7 +4824,7 @@
         <v>123</v>
       </c>
       <c r="F36" s="52" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G36" s="53">
         <v>1</v>
@@ -4881,16 +4885,16 @@
     <row r="37" spans="1:24" s="100" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B37" s="4"/>
       <c r="C37" s="56" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="D37" s="56" t="s">
         <v>117</v>
       </c>
-      <c r="E37" s="104" t="s">
+      <c r="E37" s="103" t="s">
+        <v>259</v>
+      </c>
+      <c r="F37" s="27" t="s">
         <v>260</v>
-      </c>
-      <c r="F37" s="27" t="s">
-        <v>261</v>
       </c>
       <c r="G37" s="56">
         <v>1</v>
@@ -4901,21 +4905,33 @@
       </c>
       <c r="I37" s="56"/>
       <c r="J37" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="K37" s="19" t="s">
         <v>262</v>
-      </c>
-      <c r="K37" s="19" t="s">
-        <v>263</v>
       </c>
       <c r="L37" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="23"/>
-      <c r="P37" s="23"/>
+      <c r="M37" s="5">
+        <v>100</v>
+      </c>
+      <c r="N37" s="5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="O37" s="23">
+        <v>20</v>
+      </c>
+      <c r="P37" s="23">
+        <f t="shared" si="1"/>
+        <v>2000</v>
+      </c>
       <c r="Q37" s="18"/>
       <c r="R37" s="49"/>
-      <c r="S37" s="62"/>
+      <c r="S37" s="62" t="s">
+        <v>146</v>
+      </c>
       <c r="T37" s="46">
         <f>G37*$T$4</f>
         <v>4</v>
@@ -4930,16 +4946,16 @@
         <v>32</v>
       </c>
       <c r="C38" s="53" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D38" s="53" t="s">
         <v>174</v>
       </c>
       <c r="E38" s="47" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F38" s="52" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G38" s="53">
         <v>2</v>
@@ -4952,7 +4968,7 @@
         <v>2</v>
       </c>
       <c r="J38" s="52" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K38" s="53" t="s">
         <v>128</v>
@@ -4975,10 +4991,10 @@
         <v>1000</v>
       </c>
       <c r="Q38" s="47" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="R38" s="49" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="S38" s="62" t="s">
         <v>146</v>
@@ -5004,16 +5020,16 @@
         <v>33</v>
       </c>
       <c r="C39" s="53" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D39" s="53" t="s">
         <v>174</v>
       </c>
       <c r="E39" s="47" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F39" s="52" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G39" s="53">
         <v>1</v>
@@ -5049,10 +5065,10 @@
         <v>800</v>
       </c>
       <c r="Q39" s="47" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="R39" s="49" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="S39" s="62" t="s">
         <v>146</v>
@@ -5078,7 +5094,7 @@
         <v>34</v>
       </c>
       <c r="C40" s="53" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D40" s="53" t="s">
         <v>172</v>
@@ -5087,7 +5103,7 @@
         <v>171</v>
       </c>
       <c r="F40" s="52" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G40" s="53">
         <v>1</v>
@@ -5104,7 +5120,7 @@
         <v>173</v>
       </c>
       <c r="L40" s="50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M40" s="52">
         <v>910</v>
@@ -5170,7 +5186,7 @@
       </c>
       <c r="I41" s="53"/>
       <c r="J41" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="K41" s="19" t="s">
         <v>21</v>
@@ -5215,7 +5231,7 @@
         <v>40</v>
       </c>
       <c r="F42" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G42" s="87">
         <v>1</v>
@@ -5226,7 +5242,7 @@
       </c>
       <c r="I42" s="53"/>
       <c r="J42" s="27" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K42" s="19" t="s">
         <v>16</v>
@@ -5245,10 +5261,10 @@
         <v>0</v>
       </c>
       <c r="Q42" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="R42" s="49" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="S42" s="92"/>
       <c r="T42" s="46"/>
@@ -5282,7 +5298,7 @@
       </c>
       <c r="I43" s="53"/>
       <c r="J43" s="27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K43" s="19" t="s">
         <v>21</v>
@@ -5318,7 +5334,7 @@
         <v>38</v>
       </c>
       <c r="C44" s="44" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D44" s="35" t="s">
         <v>134</v>
@@ -5327,7 +5343,7 @@
         <v>134</v>
       </c>
       <c r="F44" s="75" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G44" s="76">
         <v>4</v>
@@ -5338,10 +5354,10 @@
       </c>
       <c r="I44" s="76"/>
       <c r="J44" s="90" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K44" s="34" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L44" s="35" t="s">
         <v>134</v>
@@ -5357,10 +5373,10 @@
         <v>0</v>
       </c>
       <c r="Q44" s="86" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="R44" s="99" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="S44" s="92"/>
       <c r="T44" s="88"/>
@@ -5372,16 +5388,16 @@
     <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="B45" s="11"/>
       <c r="C45" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F45" s="77" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G45" s="39">
         <v>3</v>
@@ -5432,16 +5448,16 @@
     <row r="46" spans="1:24" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="42"/>
       <c r="C46" s="21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D46" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="E46" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="F46" s="78" t="s">
         <v>204</v>
-      </c>
-      <c r="E46" s="21" t="s">
-        <v>201</v>
-      </c>
-      <c r="F46" s="78" t="s">
-        <v>205</v>
       </c>
       <c r="G46" s="79">
         <f>3*4*2</f>
@@ -5499,11 +5515,11 @@
       <c r="M47" s="2"/>
       <c r="N47" s="3">
         <f>SUM(N6:N44)</f>
-        <v>21080</v>
+        <v>21180</v>
       </c>
       <c r="P47" s="3">
         <f>SUM(P6:P44)</f>
-        <v>47010</v>
+        <v>49010</v>
       </c>
       <c r="V47" s="3"/>
       <c r="W47" s="3">
@@ -5618,7 +5634,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H5" s="33" t="s">
         <v>186</v>
@@ -5628,17 +5644,17 @@
       </c>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B6" s="103">
+      <c r="B6" s="104">
         <v>1</v>
       </c>
-      <c r="C6" s="103" t="s">
+      <c r="C6" s="104" t="s">
         <v>152</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>155</v>
       </c>
       <c r="E6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F6" s="19" t="s">
         <v>117</v>
@@ -5654,31 +5670,31 @@
         <v>700</v>
       </c>
       <c r="J6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B7" s="103"/>
-      <c r="C7" s="103"/>
+      <c r="B7" s="104"/>
+      <c r="C7" s="104"/>
       <c r="D7" s="17" t="s">
         <v>156</v>
       </c>
       <c r="E7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>117</v>
       </c>
       <c r="J7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="R7" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B8" s="103"/>
-      <c r="C8" s="103"/>
+      <c r="B8" s="104"/>
+      <c r="C8" s="104"/>
       <c r="D8" s="17" t="s">
         <v>157</v>
       </c>
@@ -5687,10 +5703,10 @@
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B9" s="103">
+      <c r="B9" s="104">
         <v>2</v>
       </c>
-      <c r="C9" s="103" t="s">
+      <c r="C9" s="104" t="s">
         <v>153</v>
       </c>
       <c r="D9" s="17" t="s">
@@ -5704,8 +5720,8 @@
       </c>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B10" s="103"/>
-      <c r="C10" s="103"/>
+      <c r="B10" s="104"/>
+      <c r="C10" s="104"/>
       <c r="D10" s="17" t="s">
         <v>156</v>
       </c>
@@ -5714,10 +5730,10 @@
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B11" s="103">
+      <c r="B11" s="104">
         <v>3</v>
       </c>
-      <c r="C11" s="103" t="s">
+      <c r="C11" s="104" t="s">
         <v>154</v>
       </c>
       <c r="D11" s="17" t="s">
@@ -5727,12 +5743,12 @@
         <v>117</v>
       </c>
       <c r="R11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B12" s="103"/>
-      <c r="C12" s="103"/>
+      <c r="B12" s="104"/>
+      <c r="C12" s="104"/>
       <c r="D12" s="17" t="s">
         <v>156</v>
       </c>
@@ -5740,12 +5756,12 @@
         <v>117</v>
       </c>
       <c r="S12" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B13" s="103"/>
-      <c r="C13" s="103"/>
+      <c r="B13" s="104"/>
+      <c r="C13" s="104"/>
       <c r="D13" s="17" t="s">
         <v>157</v>
       </c>

</xml_diff>